<commit_message>
updated tests and benchmarks
</commit_message>
<xml_diff>
--- a/trunk/plugins/org.eclipse.emf.henshin.tests/giraph-tests/benchmarks/sierpinski.xlsx
+++ b/trunk/plugins/org.eclipse.emf.henshin.tests/giraph-tests/benchmarks/sierpinski.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Sierpinski Benchmark in Giraph</t>
   </si>
@@ -24,19 +24,10 @@
     <t>Level</t>
   </si>
   <si>
-    <t>1 Worker</t>
-  </si>
-  <si>
     <t>2 Workers</t>
   </si>
   <si>
-    <t>3 Workers</t>
-  </si>
-  <si>
     <t>4 Workers</t>
-  </si>
-  <si>
-    <t>5 Workers</t>
   </si>
   <si>
     <t>6 Workers</t>
@@ -57,10 +48,25 @@
     <t>Level 14</t>
   </si>
   <si>
-    <t>1-12</t>
+    <t>The following table shows the level runtimes in seconds for different number of workers.</t>
   </si>
   <si>
-    <t>The following table shows the level runtimes in seconds for different number of workers.</t>
+    <t>8 Workers</t>
+  </si>
+  <si>
+    <t>10 Workers</t>
+  </si>
+  <si>
+    <t>12 Workers</t>
+  </si>
+  <si>
+    <t>Levels 1-12</t>
+  </si>
+  <si>
+    <t>Level 13</t>
+  </si>
+  <si>
+    <t>Level 15</t>
   </si>
 </sst>
 </file>
@@ -190,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -205,6 +211,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -272,22 +280,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>28.045000000000002</c:v>
+                  <c:v>25.990400000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.150600000000001</c:v>
+                  <c:v>24.3734</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.155999999999999</c:v>
+                  <c:v>26.342599999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.899000000000001</c:v>
+                  <c:v>29.321199999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.006799999999995</c:v>
+                  <c:v>32.063000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.363799999999998</c:v>
+                  <c:v>34.7834</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -315,22 +323,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>167.57839999999999</c:v>
+                  <c:v>108.98339999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102.1524</c:v>
+                  <c:v>78.215600000000009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75.879199999999997</c:v>
+                  <c:v>69.054000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63.355399999999996</c:v>
+                  <c:v>61.429400000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57.140999999999998</c:v>
+                  <c:v>59.3048</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52.993600000000008</c:v>
+                  <c:v>60.03840000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -345,11 +353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="184174848"/>
-        <c:axId val="135303168"/>
+        <c:axId val="145849344"/>
+        <c:axId val="145855616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="184174848"/>
+        <c:axId val="145849344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -384,7 +392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135303168"/>
+        <c:crossAx val="145855616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -392,7 +400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135303168"/>
+        <c:axId val="145855616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -429,7 +437,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="184174848"/>
+        <c:crossAx val="145849344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -476,17 +484,7 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.14497462817147858"/>
-          <c:y val="5.1400554097404488E-2"/>
-          <c:w val="0.82446981627296589"/>
-          <c:h val="0.76222586759988331"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -495,9 +493,44 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Level 1-12</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$A$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Levels 1-12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$45:$G$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$46:$G$46</c:f>
@@ -505,22 +538,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>28.045000000000002</c:v>
+                  <c:v>25.990400000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.150600000000001</c:v>
+                  <c:v>24.3734</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.155999999999999</c:v>
+                  <c:v>26.342599999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.899000000000001</c:v>
+                  <c:v>29.321199999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.006799999999995</c:v>
+                  <c:v>32.063000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.363799999999998</c:v>
+                  <c:v>34.7834</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -530,9 +563,44 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Level 13</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Level 13</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$45:$G$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$47:$G$47</c:f>
@@ -540,22 +608,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>31.998000000000001</c:v>
+                  <c:v>19.978999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0428</c:v>
+                  <c:v>13.783200000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.0626</c:v>
+                  <c:v>11.479799999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.3712</c:v>
+                  <c:v>8.8948</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.1733999999999991</c:v>
+                  <c:v>7.7283999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.6986000000000008</c:v>
+                  <c:v>7.2808000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -565,9 +633,44 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Level 14</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$A$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Level 14</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$45:$G$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$B$48:$G$48</c:f>
@@ -575,22 +678,92 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>107.5354</c:v>
+                  <c:v>63.014000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.959000000000003</c:v>
+                  <c:v>40.058999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>38.660599999999995</c:v>
+                  <c:v>31.2316</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.0852</c:v>
+                  <c:v>23.2134</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.960799999999999</c:v>
+                  <c:v>19.513400000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.9312</c:v>
+                  <c:v>17.9742</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Level 15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$45:$G$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$49:$G$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>181.6206</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120.4158</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.566399999999987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.654200000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>57.318800000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51.877000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -606,11 +779,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="233943424"/>
-        <c:axId val="233944960"/>
+        <c:axId val="125342080"/>
+        <c:axId val="125344000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="233943424"/>
+        <c:axId val="125342080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,10 +808,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233944960"/>
+        <c:crossAx val="125344000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -646,9 +820,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="233944960"/>
+        <c:axId val="125344000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -668,47 +843,28 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> </a:t>
+                  <a:t> time in seconds</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>times in seconds</a:t>
-                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="2.2222222222222223E-2"/>
-              <c:y val="0.14615923009623796"/>
-            </c:manualLayout>
-          </c:layout>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233943424"/>
+        <c:crossAx val="125342080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.8125564304461943"/>
-          <c:y val="5.4979585885097708E-2"/>
-          <c:w val="0.16244356955380576"/>
-          <c:h val="0.24189231554389035"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="1"/>
+      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -756,20 +912,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>771525</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>895350</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1076,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1254,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1115,13 +1271,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1129,22 +1285,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="3">
-        <v>1184.2</v>
+        <v>1323.2</v>
       </c>
       <c r="C7" s="3">
-        <v>1476.2</v>
+        <v>1725.2</v>
       </c>
       <c r="D7" s="3">
-        <v>1579.8</v>
+        <v>2094</v>
       </c>
       <c r="E7" s="3">
-        <v>1708.4</v>
+        <v>2406.4</v>
       </c>
       <c r="F7" s="3">
-        <v>1879.6</v>
+        <v>2605</v>
       </c>
       <c r="G7" s="4">
-        <v>1996.2</v>
+        <v>3015.8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1152,22 +1308,22 @@
         <v>2</v>
       </c>
       <c r="B8" s="3">
-        <v>957.6</v>
+        <v>1305.5999999999999</v>
       </c>
       <c r="C8" s="3">
-        <v>1328.8</v>
+        <v>1619.6</v>
       </c>
       <c r="D8" s="3">
-        <v>1502.6</v>
+        <v>2118.4</v>
       </c>
       <c r="E8" s="3">
-        <v>1559.8</v>
+        <v>2133.1999999999998</v>
       </c>
       <c r="F8" s="3">
-        <v>1961</v>
+        <v>2473.6</v>
       </c>
       <c r="G8" s="4">
-        <v>1855.8</v>
+        <v>2697.4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1175,22 +1331,22 @@
         <v>3</v>
       </c>
       <c r="B9" s="3">
-        <v>975.8</v>
+        <v>1295.5999999999999</v>
       </c>
       <c r="C9" s="3">
-        <v>1266</v>
+        <v>1531.6</v>
       </c>
       <c r="D9" s="3">
-        <v>1622.4</v>
+        <v>1925.4</v>
       </c>
       <c r="E9" s="3">
-        <v>1684.2</v>
+        <v>2187</v>
       </c>
       <c r="F9" s="3">
-        <v>1933.8</v>
+        <v>2463.4</v>
       </c>
       <c r="G9" s="4">
-        <v>1801.6</v>
+        <v>3026</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1198,22 +1354,22 @@
         <v>4</v>
       </c>
       <c r="B10" s="3">
-        <v>1015.6</v>
+        <v>1416.6</v>
       </c>
       <c r="C10" s="3">
-        <v>1299.4000000000001</v>
+        <v>1541</v>
       </c>
       <c r="D10" s="3">
-        <v>1567.2</v>
+        <v>1868</v>
       </c>
       <c r="E10" s="3">
-        <v>1580.8</v>
+        <v>2145.6</v>
       </c>
       <c r="F10" s="3">
-        <v>1655.8</v>
+        <v>2465.4</v>
       </c>
       <c r="G10" s="4">
-        <v>1828.6</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1221,22 +1377,22 @@
         <v>5</v>
       </c>
       <c r="B11" s="3">
-        <v>954.4</v>
+        <v>1348.8</v>
       </c>
       <c r="C11" s="3">
-        <v>1307</v>
+        <v>1629.6</v>
       </c>
       <c r="D11" s="3">
-        <v>1646.6</v>
+        <v>1709</v>
       </c>
       <c r="E11" s="3">
-        <v>1629.4</v>
+        <v>2104.8000000000002</v>
       </c>
       <c r="F11" s="3">
-        <v>1705.4</v>
+        <v>2418.4</v>
       </c>
       <c r="G11" s="4">
-        <v>2015.6</v>
+        <v>2597.1999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1244,22 +1400,22 @@
         <v>6</v>
       </c>
       <c r="B12" s="3">
-        <v>1025.5999999999999</v>
+        <v>1384.2</v>
       </c>
       <c r="C12" s="3">
-        <v>1292.8</v>
+        <v>1576.2</v>
       </c>
       <c r="D12" s="3">
-        <v>1529</v>
+        <v>1689.4</v>
       </c>
       <c r="E12" s="3">
-        <v>1571.8</v>
+        <v>2160</v>
       </c>
       <c r="F12" s="3">
-        <v>1704.4</v>
+        <v>2431.4</v>
       </c>
       <c r="G12" s="4">
-        <v>1814.8</v>
+        <v>2559.1999999999998</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1267,22 +1423,22 @@
         <v>7</v>
       </c>
       <c r="B13" s="3">
-        <v>1231.4000000000001</v>
+        <v>1348.2</v>
       </c>
       <c r="C13" s="3">
-        <v>1324</v>
+        <v>1610.4</v>
       </c>
       <c r="D13" s="3">
-        <v>1438.2</v>
+        <v>1755</v>
       </c>
       <c r="E13" s="3">
-        <v>1755.2</v>
+        <v>2186.4</v>
       </c>
       <c r="F13" s="3">
-        <v>1800.8</v>
+        <v>2455.6</v>
       </c>
       <c r="G13" s="4">
-        <v>1841.4</v>
+        <v>2698.6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1290,22 +1446,22 @@
         <v>8</v>
       </c>
       <c r="B14" s="3">
-        <v>1344.4</v>
+        <v>1466.8</v>
       </c>
       <c r="C14" s="3">
-        <v>1559</v>
+        <v>1571</v>
       </c>
       <c r="D14" s="3">
-        <v>1512.6</v>
+        <v>1757.8</v>
       </c>
       <c r="E14" s="3">
-        <v>1662.2</v>
+        <v>2131.6</v>
       </c>
       <c r="F14" s="3">
-        <v>1837.4</v>
+        <v>2538</v>
       </c>
       <c r="G14" s="4">
-        <v>1860.8</v>
+        <v>2518.1999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1313,22 +1469,22 @@
         <v>9</v>
       </c>
       <c r="B15" s="3">
-        <v>1384.4</v>
+        <v>1555</v>
       </c>
       <c r="C15" s="3">
-        <v>1803.4</v>
+        <v>1832.4</v>
       </c>
       <c r="D15" s="3">
-        <v>1715.6</v>
+        <v>1877</v>
       </c>
       <c r="E15" s="3">
-        <v>1753.6</v>
+        <v>2244.8000000000002</v>
       </c>
       <c r="F15" s="3">
-        <v>1884.6</v>
+        <v>2467</v>
       </c>
       <c r="G15" s="4">
-        <v>1937.6</v>
+        <v>2899.8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1336,22 +1492,22 @@
         <v>10</v>
       </c>
       <c r="B16" s="3">
-        <v>2135.6</v>
+        <v>2027.8</v>
       </c>
       <c r="C16" s="3">
-        <v>1921.2</v>
+        <v>1923</v>
       </c>
       <c r="D16" s="3">
-        <v>1874.2</v>
+        <v>2267.4</v>
       </c>
       <c r="E16" s="3">
-        <v>1939.8</v>
+        <v>2619</v>
       </c>
       <c r="F16" s="3">
-        <v>2034.6</v>
+        <v>2725.4</v>
       </c>
       <c r="G16" s="4">
-        <v>2138.4</v>
+        <v>2826.2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1359,22 +1515,22 @@
         <v>11</v>
       </c>
       <c r="B17" s="3">
-        <v>4300</v>
+        <v>3737.4</v>
       </c>
       <c r="C17" s="3">
-        <v>3376.8</v>
+        <v>2604.4</v>
       </c>
       <c r="D17" s="3">
-        <v>2766.8</v>
+        <v>2613.6</v>
       </c>
       <c r="E17" s="3">
-        <v>2479.1999999999998</v>
+        <v>2888.6</v>
       </c>
       <c r="F17" s="3">
-        <v>2531.8000000000002</v>
+        <v>3007.8</v>
       </c>
       <c r="G17" s="4">
-        <v>2541.4</v>
+        <v>3308</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1382,22 +1538,22 @@
         <v>12</v>
       </c>
       <c r="B18" s="3">
-        <v>11536</v>
+        <v>7781.2</v>
       </c>
       <c r="C18" s="3">
-        <v>7196</v>
+        <v>5209</v>
       </c>
       <c r="D18" s="3">
-        <v>5401</v>
+        <v>4667.6000000000004</v>
       </c>
       <c r="E18" s="3">
-        <v>4574.6000000000004</v>
+        <v>4113.8</v>
       </c>
       <c r="F18" s="3">
-        <v>4077.6</v>
+        <v>4012</v>
       </c>
       <c r="G18" s="4">
-        <v>3731.6</v>
+        <v>4073</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1405,22 +1561,22 @@
         <v>13</v>
       </c>
       <c r="B19" s="3">
-        <v>31998</v>
+        <v>19979</v>
       </c>
       <c r="C19" s="3">
-        <v>20042.8</v>
+        <v>13783.2</v>
       </c>
       <c r="D19" s="3">
-        <v>13062.6</v>
+        <v>11479.8</v>
       </c>
       <c r="E19" s="3">
-        <v>10371.200000000001</v>
+        <v>8894.7999999999993</v>
       </c>
       <c r="F19" s="3">
-        <v>9173.4</v>
+        <v>7728.4</v>
       </c>
       <c r="G19" s="4">
-        <v>7698.6</v>
+        <v>7280.8</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1428,241 +1584,282 @@
         <v>14</v>
       </c>
       <c r="B20" s="6">
-        <v>107535.4</v>
+        <v>63014</v>
       </c>
       <c r="C20" s="6">
-        <v>56959</v>
+        <v>40059</v>
       </c>
       <c r="D20" s="6">
-        <v>38660.6</v>
+        <v>31231.599999999999</v>
       </c>
       <c r="E20" s="6">
-        <v>29085.200000000001</v>
+        <v>23213.4</v>
       </c>
       <c r="F20" s="6">
-        <v>22960.799999999999</v>
+        <v>19513.400000000001</v>
       </c>
       <c r="G20" s="7">
-        <v>19931.2</v>
+        <v>17974.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>181620.6</v>
+      </c>
+      <c r="C21">
+        <v>120415.8</v>
+      </c>
+      <c r="D21">
+        <v>96566.399999999994</v>
+      </c>
+      <c r="E21">
+        <v>68654.2</v>
+      </c>
+      <c r="F21">
+        <v>57318.8</v>
+      </c>
+      <c r="G21">
+        <v>51877</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" s="3">
         <f>SUM(B7:B18)/1000</f>
-        <v>28.045000000000002</v>
+        <v>25.990400000000001</v>
       </c>
       <c r="C26" s="4">
         <f>SUM(B7:B20)/1000</f>
-        <v>167.57839999999999</v>
+        <v>108.98339999999999</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B27" s="3">
         <f>SUM(C7:C18)/1000</f>
-        <v>25.150600000000001</v>
+        <v>24.3734</v>
       </c>
       <c r="C27" s="4">
         <f>SUM(C7:C20)/1000</f>
-        <v>102.1524</v>
+        <v>78.215600000000009</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B28" s="3">
         <f>SUM(D7:D18)/1000</f>
-        <v>24.155999999999999</v>
+        <v>26.342599999999997</v>
       </c>
       <c r="C28" s="4">
         <f>SUM(D7:D20)/1000</f>
-        <v>75.879199999999997</v>
+        <v>69.054000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B29" s="3">
         <f>SUM(E7:E18)/1000</f>
-        <v>23.899000000000001</v>
+        <v>29.321199999999997</v>
       </c>
       <c r="C29" s="4">
         <f>SUM(E7:E20)/1000</f>
-        <v>63.355399999999996</v>
+        <v>61.429400000000001</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B30" s="3">
         <f>SUM(F7:F18)/1000</f>
-        <v>25.006799999999995</v>
+        <v>32.063000000000002</v>
       </c>
       <c r="C30" s="4">
         <f>SUM(F7:F20)/1000</f>
-        <v>57.140999999999998</v>
+        <v>59.3048</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B31" s="6">
         <f>SUM(G7:G18)/1000</f>
-        <v>25.363799999999998</v>
+        <v>34.7834</v>
       </c>
       <c r="C31" s="7">
         <f>SUM(G7:G20)/1000</f>
-        <v>52.993600000000008</v>
+        <v>60.03840000000001</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" s="9" t="s">
+      <c r="A45" s="8"/>
+      <c r="B45" s="9">
         <v>2</v>
       </c>
-      <c r="C45" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="9" t="s">
+      <c r="C45" s="9">
         <v>4</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" s="9" t="s">
+      <c r="D45" s="9">
         <v>6</v>
       </c>
-      <c r="G45" s="10" t="s">
-        <v>7</v>
+      <c r="E45" s="9">
+        <v>8</v>
+      </c>
+      <c r="F45" s="9">
+        <v>10</v>
+      </c>
+      <c r="G45" s="10">
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B46" s="3">
-        <f>SUM(B7:B18)/1000</f>
-        <v>28.045000000000002</v>
+        <f t="shared" ref="B46:G46" si="0">SUM(B7:B18)/1000</f>
+        <v>25.990400000000001</v>
       </c>
       <c r="C46" s="3">
-        <f>SUM(C7:C18)/1000</f>
-        <v>25.150600000000001</v>
+        <f t="shared" si="0"/>
+        <v>24.3734</v>
       </c>
       <c r="D46" s="3">
-        <f>SUM(D7:D18)/1000</f>
-        <v>24.155999999999999</v>
+        <f t="shared" si="0"/>
+        <v>26.342599999999997</v>
       </c>
       <c r="E46" s="3">
-        <f>SUM(E7:E18)/1000</f>
-        <v>23.899000000000001</v>
+        <f t="shared" si="0"/>
+        <v>29.321199999999997</v>
       </c>
       <c r="F46" s="13">
-        <f>SUM(F7:F18)/1000</f>
-        <v>25.006799999999995</v>
+        <f t="shared" si="0"/>
+        <v>32.063000000000002</v>
       </c>
       <c r="G46" s="4">
-        <f>SUM(G7:G18)/1000</f>
-        <v>25.363799999999998</v>
+        <f t="shared" si="0"/>
+        <v>34.7834</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
-        <v>13</v>
+      <c r="A47" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="B47" s="3">
         <f>B19/1000</f>
-        <v>31.998000000000001</v>
+        <v>19.978999999999999</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" ref="C47:G47" si="0">C19/1000</f>
-        <v>20.0428</v>
+        <f t="shared" ref="C47:G47" si="1">C19/1000</f>
+        <v>13.783200000000001</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" si="0"/>
-        <v>13.0626</v>
+        <f t="shared" si="1"/>
+        <v>11.479799999999999</v>
       </c>
       <c r="E47" s="3">
-        <f t="shared" si="0"/>
-        <v>10.3712</v>
+        <f t="shared" si="1"/>
+        <v>8.8948</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" si="0"/>
-        <v>9.1733999999999991</v>
+        <f t="shared" si="1"/>
+        <v>7.7283999999999997</v>
       </c>
       <c r="G47" s="4">
-        <f t="shared" si="0"/>
-        <v>7.6986000000000008</v>
+        <f t="shared" si="1"/>
+        <v>7.2808000000000002</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="12">
-        <v>14</v>
+      <c r="A48" s="12" t="s">
+        <v>9</v>
       </c>
       <c r="B48" s="6">
         <f>B20/1000</f>
-        <v>107.5354</v>
+        <v>63.014000000000003</v>
       </c>
       <c r="C48" s="6">
-        <f t="shared" ref="C48:G48" si="1">C20/1000</f>
-        <v>56.959000000000003</v>
+        <f t="shared" ref="C48:G49" si="2">C20/1000</f>
+        <v>40.058999999999997</v>
       </c>
       <c r="D48" s="6">
-        <f t="shared" si="1"/>
-        <v>38.660599999999995</v>
+        <f t="shared" si="2"/>
+        <v>31.2316</v>
       </c>
       <c r="E48" s="6">
-        <f t="shared" si="1"/>
-        <v>29.0852</v>
+        <f t="shared" si="2"/>
+        <v>23.2134</v>
       </c>
       <c r="F48" s="6">
-        <f t="shared" si="1"/>
-        <v>22.960799999999999</v>
+        <f t="shared" si="2"/>
+        <v>19.513400000000001</v>
       </c>
       <c r="G48" s="7">
-        <f t="shared" si="1"/>
-        <v>19.9312</v>
+        <f t="shared" si="2"/>
+        <v>17.9742</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
+      <c r="A49" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="6">
+        <f>B21/1000</f>
+        <v>181.6206</v>
+      </c>
+      <c r="C49" s="6">
+        <f t="shared" si="2"/>
+        <v>120.4158</v>
+      </c>
+      <c r="D49" s="6">
+        <f t="shared" si="2"/>
+        <v>96.566399999999987</v>
+      </c>
+      <c r="E49" s="6">
+        <f t="shared" si="2"/>
+        <v>68.654200000000003</v>
+      </c>
+      <c r="F49" s="6">
+        <f t="shared" si="2"/>
+        <v>57.318800000000003</v>
+      </c>
+      <c r="G49" s="7">
+        <f t="shared" si="2"/>
+        <v>51.877000000000002</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>

</xml_diff>